<commit_message>
Women Bargaining Index and Health measures
Here, I included the women bargaining index through a principal component analysis. Also, I calculated the z-scores for the height-for-age index
</commit_message>
<xml_diff>
--- a/Inputs/Codes.xlsx
+++ b/Inputs/Codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\OneDrive\Desktop\Development Economics MSc\Dissertation\R\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/500a1adc9097afdd/Desktop/Development Economics MSc/Dissertation/R/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8CE416-3C58-4DCE-A838-B1020A8FDF9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{6E8CE416-3C58-4DCE-A838-B1020A8FDF9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{79686900-1363-4DFE-AECF-C861973FC15B}"/>
   <bookViews>
-    <workbookView xWindow="31560" yWindow="3930" windowWidth="17280" windowHeight="8970" firstSheet="1" activeTab="7" xr2:uid="{6DB7C2AC-8DEC-4E03-B46D-212C674364A6}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="6" xr2:uid="{6DB7C2AC-8DEC-4E03-B46D-212C674364A6}"/>
   </bookViews>
   <sheets>
     <sheet name="c_ls" sheetId="1" r:id="rId1"/>
@@ -255,39 +255,6 @@
     <t>sequence</t>
   </si>
   <si>
-    <t>food_house</t>
-  </si>
-  <si>
-    <t>own_clothes</t>
-  </si>
-  <si>
-    <t>spouse_clothes</t>
-  </si>
-  <si>
-    <t>children_clothes</t>
-  </si>
-  <si>
-    <t>children_education</t>
-  </si>
-  <si>
-    <t>children_health</t>
-  </si>
-  <si>
-    <t>strong_expenditure</t>
-  </si>
-  <si>
-    <t>money_relatives</t>
-  </si>
-  <si>
-    <t>own_work</t>
-  </si>
-  <si>
-    <t>spouse_work</t>
-  </si>
-  <si>
-    <t>contraceptives</t>
-  </si>
-  <si>
     <t>decision</t>
   </si>
   <si>
@@ -300,9 +267,6 @@
     <t>key_dec</t>
   </si>
   <si>
-    <t>money_spo_relatives</t>
-  </si>
-  <si>
     <t>question</t>
   </si>
   <si>
@@ -511,6 +475,42 @@
   </si>
   <si>
     <t>Veracruz</t>
+  </si>
+  <si>
+    <t>Food eaten in the house</t>
+  </si>
+  <si>
+    <t>Your clothes</t>
+  </si>
+  <si>
+    <t>Your spouse's clothes</t>
+  </si>
+  <si>
+    <t>Your children's clothes</t>
+  </si>
+  <si>
+    <t>Your children's education</t>
+  </si>
+  <si>
+    <t>Your children's health</t>
+  </si>
+  <si>
+    <t>Strong expenditure</t>
+  </si>
+  <si>
+    <t>Money given to your relatives</t>
+  </si>
+  <si>
+    <t>Money given to your spouse's relatives</t>
+  </si>
+  <si>
+    <t>If you should work</t>
+  </si>
+  <si>
+    <t>If your spouse should work</t>
+  </si>
+  <si>
+    <t>Use of contraceptives</t>
   </si>
 </sst>
 </file>
@@ -1016,18 +1016,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -1060,7 +1060,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B12">
         <v>7</v>
@@ -1148,7 +1148,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1174,10 +1174,10 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1536,24 +1536,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16BFC4A-CF8B-40B0-AFE8-6EE58983651E}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1561,7 +1562,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>144</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1572,7 +1573,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1583,7 +1584,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>146</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1594,7 +1595,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>147</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1605,7 +1606,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1616,7 +1617,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>149</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1627,7 +1628,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1638,7 +1639,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>151</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1649,7 +1650,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1660,7 +1661,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1671,7 +1672,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>154</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1682,7 +1683,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>155</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1697,7 +1698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1FF772-8BC2-4149-87A2-5293DD51CD15}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -1708,16 +1709,16 @@
         <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C1" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="D1" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="E1" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1725,7 +1726,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -1742,7 +1743,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -1759,7 +1760,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C4">
         <v>7</v>
@@ -1776,7 +1777,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C5">
         <v>7</v>
@@ -1793,7 +1794,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1810,7 +1811,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1827,7 +1828,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1844,7 +1845,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C9">
         <v>7</v>
@@ -1861,7 +1862,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C10">
         <v>8</v>
@@ -1878,7 +1879,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C11">
         <v>7</v>
@@ -1895,7 +1896,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C12">
         <v>7</v>
@@ -1912,7 +1913,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -1929,7 +1930,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1946,7 +1947,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C15">
         <v>7</v>
@@ -1963,7 +1964,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -1980,7 +1981,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C17">
         <v>7</v>
@@ -1997,7 +1998,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -2014,7 +2015,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -2031,7 +2032,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C20">
         <v>7</v>
@@ -2048,7 +2049,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C21">
         <v>7</v>
@@ -2065,7 +2066,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -2082,7 +2083,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C23" s="1">
         <v>7</v>
@@ -2099,7 +2100,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C24" s="1">
         <v>6</v>
@@ -2116,7 +2117,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C25">
         <v>7</v>
@@ -2133,7 +2134,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -2150,7 +2151,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C27">
         <v>7</v>
@@ -2167,7 +2168,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C28">
         <v>7</v>
@@ -2184,7 +2185,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C29">
         <v>6</v>
@@ -2201,7 +2202,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2218,7 +2219,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C31">
         <v>7</v>
@@ -2235,7 +2236,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C32">
         <v>4</v>
@@ -2252,7 +2253,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C33">
         <v>7</v>
@@ -2281,18 +2282,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -2303,7 +2304,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -2314,7 +2315,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -2325,7 +2326,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -2336,7 +2337,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -2347,7 +2348,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -2358,7 +2359,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -2369,7 +2370,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -2380,7 +2381,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2391,7 +2392,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -2402,7 +2403,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -2413,7 +2414,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -2424,7 +2425,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -2435,7 +2436,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -2446,7 +2447,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -2457,7 +2458,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -2468,7 +2469,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -2479,7 +2480,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B19">
         <v>5</v>

</xml_diff>

<commit_message>
Unify information and codes
Include full variables of PCA  and household and individual characteristics to the main database ready for the analysis.
</commit_message>
<xml_diff>
--- a/Inputs/Codes.xlsx
+++ b/Inputs/Codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/500a1adc9097afdd/Desktop/Development Economics MSc/Dissertation/R/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{6E8CE416-3C58-4DCE-A838-B1020A8FDF9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{79686900-1363-4DFE-AECF-C861973FC15B}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{6E8CE416-3C58-4DCE-A838-B1020A8FDF9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{309BB1FB-C5DB-4FA4-BC6A-69F31DAE346F}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="6" xr2:uid="{6DB7C2AC-8DEC-4E03-B46D-212C674364A6}"/>
+    <workbookView xWindow="2580" yWindow="2148" windowWidth="17280" windowHeight="8976" activeTab="6" xr2:uid="{6DB7C2AC-8DEC-4E03-B46D-212C674364A6}"/>
   </bookViews>
   <sheets>
     <sheet name="c_ls" sheetId="1" r:id="rId1"/>
@@ -477,40 +477,40 @@
     <t>Veracruz</t>
   </si>
   <si>
-    <t>Food eaten in the house</t>
-  </si>
-  <si>
-    <t>Your clothes</t>
-  </si>
-  <si>
-    <t>Your spouse's clothes</t>
-  </si>
-  <si>
-    <t>Your children's clothes</t>
-  </si>
-  <si>
-    <t>Your children's education</t>
-  </si>
-  <si>
-    <t>Your children's health</t>
-  </si>
-  <si>
     <t>Strong expenditure</t>
   </si>
   <si>
-    <t>Money given to your relatives</t>
-  </si>
-  <si>
-    <t>Money given to your spouse's relatives</t>
-  </si>
-  <si>
-    <t>If you should work</t>
-  </si>
-  <si>
-    <t>If your spouse should work</t>
-  </si>
-  <si>
-    <t>Use of contraceptives</t>
+    <t>Food in the house</t>
+  </si>
+  <si>
+    <t>Children's clothes</t>
+  </si>
+  <si>
+    <t>Spouse's clothes</t>
+  </si>
+  <si>
+    <t>Own clothes</t>
+  </si>
+  <si>
+    <t>Children's education</t>
+  </si>
+  <si>
+    <t>Children's health</t>
+  </si>
+  <si>
+    <t>Money to spouse's relatives</t>
+  </si>
+  <si>
+    <t>Money to relatives</t>
+  </si>
+  <si>
+    <t>Own work</t>
+  </si>
+  <si>
+    <t>Spouse's work</t>
+  </si>
+  <si>
+    <t>Contraceptives</t>
   </si>
 </sst>
 </file>
@@ -1562,7 +1562,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1573,7 +1573,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1584,7 +1584,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1595,7 +1595,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1606,7 +1606,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1617,7 +1617,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1628,7 +1628,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1639,7 +1639,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1650,7 +1650,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C10">
         <v>0</v>

</xml_diff>